<commit_message>
Update 1p6. Constant Radius maneuver, optimization example
</commit_message>
<xml_diff>
--- a/Libraries/Event/sm_car_database_Driver.xlsx
+++ b/Libraries/Event/sm_car_database_Driver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Event\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0772570-4D2E-4063-A308-78E79A081723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F186F8DB-AF44-470C-81AA-44752FE8998E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="2955" windowWidth="17280" windowHeight="10215" tabRatio="889" firstSheet="17" activeTab="23" xr2:uid="{87770AAC-9142-4F0B-A47A-9193DA8A8904}"/>
+    <workbookView xWindow="1200" yWindow="852" windowWidth="13008" windowHeight="10152" tabRatio="889" firstSheet="18" activeTab="21" xr2:uid="{87770AAC-9142-4F0B-A47A-9193DA8A8904}"/>
   </bookViews>
   <sheets>
     <sheet name="Mallory_HambaLG" sheetId="1" r:id="rId1"/>
@@ -24,19 +24,26 @@
     <sheet name="CRG_Nurburgring_N_Hamba" sheetId="20" r:id="rId9"/>
     <sheet name="CRG_Suzuka_Hamba" sheetId="22" r:id="rId10"/>
     <sheet name="CRG_Mallory_Hamba" sheetId="19" r:id="rId11"/>
-    <sheet name="CRG_Pikes_Peak_Hamba" sheetId="21" r:id="rId12"/>
-    <sheet name="DLC_HambaLG" sheetId="6" r:id="rId13"/>
-    <sheet name="DLC_Hamba" sheetId="7" r:id="rId14"/>
-    <sheet name="DLC_Makhulu" sheetId="10" r:id="rId15"/>
-    <sheet name="Skidpad_HambaLG" sheetId="17" r:id="rId16"/>
-    <sheet name="Skidpad_Hamba" sheetId="16" r:id="rId17"/>
-    <sheet name="Skidpad_Makhulu" sheetId="18" r:id="rId18"/>
-    <sheet name="Str_HambaLG" sheetId="13" r:id="rId19"/>
-    <sheet name="Str_Hamba" sheetId="14" r:id="rId20"/>
-    <sheet name="Str_Makhulu" sheetId="15" r:id="rId21"/>
-    <sheet name="FTP75_HambaLG" sheetId="25" r:id="rId22"/>
-    <sheet name="FTP75_Hamba" sheetId="26" r:id="rId23"/>
-    <sheet name="FTP75_Makhulu" sheetId="27" r:id="rId24"/>
+    <sheet name="CRG_Custom" sheetId="31" r:id="rId12"/>
+    <sheet name="CRG_Pikes_Peak_Hamba" sheetId="21" r:id="rId13"/>
+    <sheet name="DLC_HambaLG" sheetId="6" r:id="rId14"/>
+    <sheet name="DLC_Hamba" sheetId="7" r:id="rId15"/>
+    <sheet name="DLC_Makhulu" sheetId="10" r:id="rId16"/>
+    <sheet name="Skidpad_HambaLG" sheetId="17" r:id="rId17"/>
+    <sheet name="Skidpad_Hamba" sheetId="16" r:id="rId18"/>
+    <sheet name="Skidpad_Makhulu" sheetId="18" r:id="rId19"/>
+    <sheet name="RadiusCL_HambaLG" sheetId="32" r:id="rId20"/>
+    <sheet name="RadiusCL_Hamba" sheetId="33" r:id="rId21"/>
+    <sheet name="RadiusCL_Makhulu" sheetId="34" r:id="rId22"/>
+    <sheet name="Str_HambaLG" sheetId="13" r:id="rId23"/>
+    <sheet name="Str_Hamba" sheetId="14" r:id="rId24"/>
+    <sheet name="Str_Makhulu" sheetId="15" r:id="rId25"/>
+    <sheet name="FTP75_HambaLG" sheetId="25" r:id="rId26"/>
+    <sheet name="FTP75_Hamba" sheetId="26" r:id="rId27"/>
+    <sheet name="FTP75_Makhulu" sheetId="27" r:id="rId28"/>
+    <sheet name="UrbanCycle1_HambaLG" sheetId="28" r:id="rId29"/>
+    <sheet name="UrbanCycle1_Hamba" sheetId="29" r:id="rId30"/>
+    <sheet name="UrbanCycle1_Makhulu" sheetId="30" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="64">
   <si>
     <t>rad/s</t>
   </si>
@@ -240,6 +247,15 @@
   <si>
     <t>Hz</t>
   </si>
+  <si>
+    <t>DriveCycle_UrbanCycle1</t>
+  </si>
+  <si>
+    <t>CRG_Custom</t>
+  </si>
+  <si>
+    <t>Constant_Radius_CL</t>
+  </si>
 </sst>
 </file>
 
@@ -309,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -345,12 +361,254 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2132,32 +2390,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="134" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="131" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="130" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="129" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2693,32 +2951,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="79" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3254,32 +3512,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="73" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3288,6 +3546,567 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C5560B-2686-4582-BFD7-2210723D3CF3}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4" s="1"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5" s="1"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+    </row>
+    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6">
+        <v>2.8239999999999998</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6" s="1"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+    </row>
+    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="6">
+        <v>80</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7" s="1"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="16">
+        <f>2*PI()*50</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="3"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8" s="1"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="H9" s="16">
+        <v>1500</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="3"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10">
+        <v>17297</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U35" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
+    <cfRule type="cellIs" dxfId="101" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="100" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B9">
+    <cfRule type="cellIs" dxfId="99" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="97" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C4">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24919A65-0CA2-414C-8049-302FA5DB3433}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -3815,32 +4634,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="68" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3848,7 +4667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F567C822-749C-412E-BF96-0F073B4A9DAE}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -4384,32 +5203,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="61" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="59" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4417,7 +5236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA27FF2-149D-4915-8E2B-EA094988B469}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -4945,32 +5764,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4978,7 +5797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD959DC-12D8-4BFA-8F52-866E2FEE629D}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -5506,32 +6325,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5539,7 +6358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA9B50F-EB1D-42F6-8596-0AE27FD43915}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -6067,32 +6886,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6100,7 +6919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F22C8C-FD12-4E89-A0A8-32924D00C83A}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -6628,32 +7447,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6661,7 +7480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75C1912-1029-4E76-B073-455C0298204A}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -7189,593 +8008,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAD4ED6-7B9B-46BE-B492-50BF3D4DFCD6}">
-  <sheetPr>
-    <tabColor theme="4" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:AA35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M35" sqref="M35"/>
-      <selection pane="topRight" activeCell="M35" sqref="M35"/>
-      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-    </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3" s="1"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-    </row>
-    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="14">
-        <v>3</v>
-      </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4" s="1"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-    </row>
-    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6">
-        <v>3</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5" s="1"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-    </row>
-    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="6">
-        <v>3.57</v>
-      </c>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6" s="1"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6">
-        <v>80</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7" s="1"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-    </row>
-    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="H8" s="16">
-        <f>2*PI()*50</f>
-        <v>314.15926535897933</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8" s="3"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="U8" s="1"/>
-      <c r="V8"/>
-    </row>
-    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="H9" s="16">
-        <v>2550</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9" s="3"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="U9" s="1"/>
-    </row>
-    <row r="10" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10"/>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10">
-        <v>17297</v>
-      </c>
-      <c r="U10" s="1"/>
-    </row>
-    <row r="11" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11"/>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11">
-        <v>0.1</v>
-      </c>
-      <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12">
-        <v>20</v>
-      </c>
-      <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13"/>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13">
-        <v>200</v>
-      </c>
-      <c r="U13" s="1"/>
-    </row>
-    <row r="14" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14"/>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14">
-        <v>2.5</v>
-      </c>
-      <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="15">
-        <v>9.8066499999999994</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="15">
-        <f>2*PI()*5</f>
-        <v>31.415926535897931</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="15">
-        <f>2*PI()*5</f>
-        <v>31.415926535897931</v>
-      </c>
-      <c r="U18" s="1"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U19" s="1"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U23" s="1"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U26" s="1"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U30" s="1"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U31" s="1"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U32" s="1"/>
-    </row>
-    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
-      <c r="U33" s="1"/>
-    </row>
-    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="1"/>
-    </row>
-    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
-      <c r="U35" s="1"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8311,32 +8569,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="128" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="127" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="126" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="125" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="124" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="123" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8345,6 +8603,1692 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B50D3F-CCFE-4E8F-A1EB-06F199148344}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:U35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="H3" sqref="H3"/>
+      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22">
+        <v>3</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="23">
+        <v>3</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="23">
+        <v>3.57</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="23">
+        <v>80</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="H8" s="18">
+        <f>2*PI()*50</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="H9" s="18">
+        <v>2550</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>17297</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U35" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B9">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C4">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59256037-4161-463D-B30D-94370CAEA18C}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:U35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="H3" sqref="H3"/>
+      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="23">
+        <v>3</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="23">
+        <v>2.8239999999999998</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="23">
+        <v>80</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="H8" s="18">
+        <f>2*PI()*50</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="H9" s="18">
+        <v>1500</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>17297</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U35" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B9">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C4">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB079F7-2FE4-4E50-A2D5-2C56A023F64D}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:U35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22">
+        <v>3</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="23">
+        <v>3</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="23">
+        <v>6.7816000000000001</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="23">
+        <v>80</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="H8" s="18">
+        <f>2*PI()*50</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="H9" s="18">
+        <v>2550</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>17297</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U35" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B9">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAD4ED6-7B9B-46BE-B492-50BF3D4DFCD6}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="14">
+        <v>3</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4" s="1"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5" s="1"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+    </row>
+    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6">
+        <v>3.57</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6" s="1"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+    </row>
+    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="6">
+        <v>80</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7" s="1"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="16">
+        <f>2*PI()*50</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="3"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8" s="1"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="H9" s="16">
+        <v>2550</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="3"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10">
+        <v>17297</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="15">
+        <f>2*PI()*5</f>
+        <v>31.415926535897931</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U35" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C7 B8 A8:A9">
+    <cfRule type="cellIs" dxfId="53" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="52" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B9">
+    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C4">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027B20D6-2BBB-48B2-8BFD-E084F702B920}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -8872,32 +10816,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8905,7 +10849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE29C2-9856-4376-B819-E5383B7B41B1}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -9433,32 +11377,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9466,7 +11410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D73856-57BF-43D4-AF71-247688B704AE}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -9698,17 +11642,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:B4">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9716,7 +11660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D7F364-89D9-4BAA-B99D-5B952DB6548F}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -9948,17 +11892,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:B4">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9966,14 +11910,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FAE147-41AA-4B7D-B476-A5629690F5D4}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M35" sqref="M35"/>
       <selection pane="topRight" activeCell="M35" sqref="M35"/>
@@ -10198,17 +12142,267 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:B4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88C32E3-E030-41F3-89E9-55E181619004}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4" s="3"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5" s="18">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="18">
+        <v>10</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="18">
+        <f>2*PI()*20</f>
+        <v>125.66370614359172</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A4:B4">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10744,32 +12938,532 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="122" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="121" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="120" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="119" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="117" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017A0C96-9492-4C12-8899-089B54D76808}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4" s="3"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5" s="18">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="18">
+        <v>10</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="18">
+        <f>2*PI()*20</f>
+        <v>125.66370614359172</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A4:B4">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990D917E-2C74-4183-ABA6-A929993A161D}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="T41" sqref="T41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4" s="3"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5" s="18">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="18">
+        <v>10</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="18">
+        <f>2*PI()*20</f>
+        <v>125.66370614359172</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A4:B4">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11305,32 +13999,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="116" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="115" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="114" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="112" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11866,32 +14560,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="110" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="109" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="108" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="107" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12427,32 +15121,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="104" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="103" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="102" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="99" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12988,32 +15682,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="98" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="96" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="94" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="93" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13549,32 +16243,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="92" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="91" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="90" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="88" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14110,32 +16804,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="86" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="85" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="84" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="83" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="82" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>